<commit_message>
fix date 25/8 - 16/9
</commit_message>
<xml_diff>
--- a/WIP/Documents/Report 1/DDL_QA_Management_Sheet_v1.0_JP.xlsx
+++ b/WIP/Documents/Report 1/DDL_QA_Management_Sheet_v1.0_JP.xlsx
@@ -602,7 +602,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="96">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1556,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2740,7 +2761,7 @@
       </c>
       <c r="C5" s="33">
         <f ca="1" xml:space="preserve"> NOW()</f>
-        <v>42264.923841203701</v>
+        <v>42264.995221296296</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="3"/>
@@ -3333,7 +3354,7 @@
       <c r="P22" s="23"/>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="1:17" s="25" customFormat="1" ht="56.25">
+    <row r="23" spans="1:17" s="25" customFormat="1" ht="45">
       <c r="A23" s="46">
         <v>10</v>
       </c>
@@ -3361,8 +3382,8 @@
       <c r="I23" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="49" t="s">
-        <v>38</v>
+      <c r="J23" s="48" t="s">
+        <v>43</v>
       </c>
       <c r="K23" s="43" t="s">
         <v>28</v>
@@ -3401,343 +3422,343 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M14:M19 O14:O19 G14 G16 G18 G20">
-    <cfRule type="expression" dxfId="92" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="97" stopIfTrue="1">
       <formula>($K14="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="98" stopIfTrue="1">
       <formula>($K14="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="99" stopIfTrue="1">
       <formula>($K14="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R20:IV20 B20:C20 N14:N15 P14:IV15 A14:F15 H14:L15 K16 P18:Q18 P17:IV17 P19:IV19 N17:N19 H17:K17 A19:A20 H18:H19 J18:K19 I21 I23 L20:L21 B17:F19">
-    <cfRule type="expression" dxfId="89" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="100" stopIfTrue="1">
       <formula>($K14="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="101" stopIfTrue="1">
       <formula>($K14="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="102" stopIfTrue="1">
       <formula>($K14="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16 P16:IV16 A16:F16 L16 H16:J16 I22 L22">
-    <cfRule type="expression" dxfId="86" priority="103" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="103" stopIfTrue="1">
       <formula>($K16="Cancelled")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="104" stopIfTrue="1">
       <formula>($K16="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="105" stopIfTrue="1">
       <formula>($K16="In Progress")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20 O20">
-    <cfRule type="expression" dxfId="83" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="91" stopIfTrue="1">
       <formula>($K20="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="92" stopIfTrue="1">
       <formula>($K20="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="93" stopIfTrue="1">
       <formula>($K20="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20 P20:Q20 D20:F20 H20 J20:K20">
-    <cfRule type="expression" dxfId="80" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="94" stopIfTrue="1">
       <formula>($K20="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="95" stopIfTrue="1">
       <formula>($K20="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="96" stopIfTrue="1">
       <formula>($K20="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:IV18">
-    <cfRule type="expression" dxfId="77" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="106" stopIfTrue="1">
       <formula>(#REF!="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="107" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="107" stopIfTrue="1">
       <formula>(#REF!="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="108" stopIfTrue="1">
       <formula>(#REF!="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="expression" dxfId="74" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="76" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="77" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="78" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P23:Q23 N23 B23:E23 H23 J23:K23">
-    <cfRule type="expression" dxfId="71" priority="79" stopIfTrue="1">
+  <conditionalFormatting sqref="P23:Q23 N23 B23:E23 H23 K23">
+    <cfRule type="expression" dxfId="74" priority="79" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="80" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="81" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23:IV23">
-    <cfRule type="expression" dxfId="68" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="151" stopIfTrue="1">
       <formula>($K18="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="152" stopIfTrue="1">
       <formula>($K18="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="153" stopIfTrue="1">
       <formula>($K18="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21 O21">
-    <cfRule type="expression" dxfId="65" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="64" stopIfTrue="1">
       <formula>($K21="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="65" stopIfTrue="1">
       <formula>($K21="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
       <formula>($K21="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21 P21:IV21 A21:H21 J21:K21">
-    <cfRule type="expression" dxfId="62" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="67" stopIfTrue="1">
       <formula>($K21="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="68" stopIfTrue="1">
       <formula>($K21="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="69" stopIfTrue="1">
       <formula>($K21="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="expression" dxfId="59" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="58" stopIfTrue="1">
       <formula>($K22="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="59" stopIfTrue="1">
       <formula>($K22="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="60" stopIfTrue="1">
       <formula>($K22="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22:IV22 A22:C22">
-    <cfRule type="expression" dxfId="56" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="61" stopIfTrue="1">
       <formula>($K22="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="62" stopIfTrue="1">
       <formula>($K22="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="63" stopIfTrue="1">
       <formula>($K22="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22 O22">
-    <cfRule type="expression" dxfId="53" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="52" stopIfTrue="1">
       <formula>($K22="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
       <formula>($K22="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="54" stopIfTrue="1">
       <formula>($K22="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N22 P22:Q22 D22:F22 H22 J22:K22">
-    <cfRule type="expression" dxfId="50" priority="55" stopIfTrue="1">
+  <conditionalFormatting sqref="N22 P22:Q22 D22:F22 H22 J22:K22 J23">
+    <cfRule type="expression" dxfId="53" priority="55" stopIfTrue="1">
       <formula>($K22="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="56" stopIfTrue="1">
       <formula>($K22="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="57" stopIfTrue="1">
       <formula>($K22="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="47" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="49" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="50" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="51" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="expression" dxfId="44" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="46" stopIfTrue="1">
       <formula>($K15="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
       <formula>($K15="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="48" stopIfTrue="1">
       <formula>($K15="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="41" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="43" stopIfTrue="1">
       <formula>($K17="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="44" stopIfTrue="1">
       <formula>($K17="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
       <formula>($K17="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="40" stopIfTrue="1">
       <formula>($K17="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
       <formula>($K17="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="42" stopIfTrue="1">
       <formula>($K17="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="expression" dxfId="35" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="37" stopIfTrue="1">
       <formula>($K17="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="38" stopIfTrue="1">
       <formula>($K17="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="39" stopIfTrue="1">
       <formula>($K17="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="34" stopIfTrue="1">
       <formula>($K19="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="35" stopIfTrue="1">
       <formula>($K19="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="36" stopIfTrue="1">
       <formula>($K19="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="31" stopIfTrue="1">
       <formula>($K19="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
       <formula>($K19="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
       <formula>($K19="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="28" stopIfTrue="1">
       <formula>($K19="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
       <formula>($K19="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="30" stopIfTrue="1">
       <formula>($K19="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="25" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="27" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="22" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
       <formula>($K20="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
       <formula>($K20="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
       <formula>($K20="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
       <formula>($K18="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
       <formula>($K18="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>($K18="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
       <formula>($K18="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>($K18="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>($K18="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>($K18="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>($K18="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>($K18="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>($K23="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>($K23="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>($K23="Cancelled")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>